<commit_message>
Sprint2 after Clarissa's changes
</commit_message>
<xml_diff>
--- a/Documentation/Product backlog+Sprint1+Sprint2.xlsx
+++ b/Documentation/Product backlog+Sprint1+Sprint2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="85">
   <si>
     <t>Developers</t>
   </si>
@@ -279,12 +279,18 @@
       <t>UI</t>
     </r>
   </si>
+  <si>
+    <t>Drag and Drop functionality</t>
+  </si>
+  <si>
+    <t>Check email validity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +381,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -426,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -455,6 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +774,8 @@
   <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T97" sqref="T97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,10 +2311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L91" sqref="L91"/>
+    <sheetView tabSelected="1" topLeftCell="C73" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,11 +2371,11 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D2">
-        <f>C2-(SUMIF(F2:F184,"=JB",G2:G184))</f>
-        <v>-8</v>
+        <f>C2-(SUMIF(F2:F176,"=JB",G2:G176))</f>
+        <v>-1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -2377,27 +2392,27 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D3">
-        <f>C3-(SUMIF(F2:F184,"=CS",G2:G184))+D29</f>
+        <f>C3-(SUMIF(F2:F176,"=CS",G2:G176))+D29</f>
         <v>-3</v>
       </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
+      <c r="E3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="14">
+        <v>5</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
         <f>G3-H3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -2409,27 +2424,27 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <f>C4-(SUMIF(F2:F184,"=IL",G2:G184))</f>
-        <v>-4</v>
+        <f>C4-(SUMIF(F2:F176,"=IL",G2:G176))</f>
+        <v>-5</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H4" s="14">
         <v>0</v>
       </c>
       <c r="I4" s="14">
         <f>G4-H4</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -2438,7 +2453,7 @@
         <v>47</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G5" s="14">
         <v>1</v>
@@ -2453,53 +2468,53 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14">
-        <f>G6-H6</f>
-        <v>1</v>
-      </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="4"/>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>G8-H8</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
+      <c r="E9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
+      <c r="H9" s="14">
         <v>0</v>
       </c>
       <c r="I9">
         <f>G9-H9</f>
-        <v>2</v>
-      </c>
-      <c r="J9" s="4">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J9" s="4"/>
       <c r="L9" s="20"/>
       <c r="M9" s="21"/>
     </row>
@@ -2508,7 +2523,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="14">
         <v>1</v>
@@ -2525,50 +2540,52 @@
       <c r="M10" s="20"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="14">
-        <v>1</v>
-      </c>
-      <c r="H11" s="14">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>G8-H8</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="4">
+        <v>5</v>
+      </c>
+    </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="E13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="14">
         <v>5</v>
       </c>
+      <c r="H13" s="14">
+        <v>0</v>
+      </c>
+      <c r="I13" s="14">
+        <f>G13-H13</f>
+        <v>5</v>
+      </c>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E14" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G14" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H14" s="14">
         <v>0</v>
       </c>
       <c r="I14" s="14">
         <f>G14-H14</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J14" s="4"/>
     </row>
@@ -2577,7 +2594,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G15" s="14">
         <v>1</v>
@@ -2592,65 +2609,64 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="14">
-        <v>1</v>
-      </c>
-      <c r="H16" s="14">
-        <v>0</v>
-      </c>
-      <c r="I16" s="14">
-        <f>G16-H16</f>
-        <v>1</v>
-      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="4"/>
+      <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="8">
+        <v>2</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <f>G18-H18</f>
+        <v>2</v>
+      </c>
+      <c r="J18" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="8" t="s">
-        <v>70</v>
+      <c r="E19" t="s">
+        <v>46</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="8">
-        <v>2</v>
-      </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="8">
-        <f>G19-H19</f>
-        <v>2</v>
-      </c>
-      <c r="J19" s="4">
-        <v>7</v>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="14">
+        <f>G20-H20</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-      <c r="H20">
+      <c r="E20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1</v>
+      </c>
+      <c r="H20" s="14">
         <v>0</v>
       </c>
       <c r="I20" s="14">
@@ -2663,7 +2679,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G21" s="14">
         <v>1</v>
@@ -2672,156 +2688,157 @@
         <v>0</v>
       </c>
       <c r="I21" s="14">
-        <f>G22-H22</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E22" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="14">
-        <v>1</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0</v>
-      </c>
-      <c r="I22" s="14">
-        <f>G23-H23</f>
-        <v>0</v>
+        <f>G21-H21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="4">
-        <v>8</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="14">
+        <f>G24-H24</f>
+        <v>2</v>
+      </c>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25">
+      <c r="E25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="14">
+        <v>5</v>
+      </c>
+      <c r="H25" s="14">
         <v>0</v>
       </c>
       <c r="I25" s="14">
         <f>G25-H25</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H26" s="14">
         <v>0</v>
       </c>
       <c r="I26" s="14">
         <f>G26-H26</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G27" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H27" s="14">
         <v>0</v>
       </c>
       <c r="I27" s="14">
         <f>G27-H27</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E28" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="14">
-        <v>1</v>
-      </c>
-      <c r="H28" s="14">
-        <v>0</v>
-      </c>
-      <c r="I28" s="14">
-        <f>G28-H28</f>
-        <v>1</v>
-      </c>
-      <c r="J28" s="4"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J29" s="9"/>
+      <c r="E29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="4">
-        <v>8</v>
-      </c>
+      <c r="E30" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="14">
+        <v>4</v>
+      </c>
+      <c r="H30" s="14">
+        <v>0</v>
+      </c>
+      <c r="I30" s="14">
+        <f>G30-H30</f>
+        <v>4</v>
+      </c>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="14" t="s">
-        <v>54</v>
+      <c r="E31" t="s">
+        <v>45</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="14">
-        <v>3</v>
-      </c>
-      <c r="H31" s="14">
-        <v>0</v>
-      </c>
-      <c r="I31" s="14">
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <f>G31-H31</f>
         <v>3</v>
       </c>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>45</v>
+      <c r="E32" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
+      <c r="G32" s="14">
+        <v>3</v>
+      </c>
+      <c r="H32" s="14">
+        <v>0</v>
+      </c>
+      <c r="I32" s="14">
         <f>G32-H32</f>
         <v>3</v>
       </c>
@@ -2829,20 +2846,20 @@
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G33" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H33" s="14">
         <v>0</v>
       </c>
       <c r="I33" s="14">
         <f>G33-H33</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J33" s="4"/>
     </row>
@@ -2851,7 +2868,7 @@
         <v>47</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G34" s="14">
         <v>1</v>
@@ -2866,98 +2883,97 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="14" t="s">
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J36" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="14">
-        <v>1</v>
-      </c>
-      <c r="H35" s="14">
-        <v>0</v>
-      </c>
-      <c r="I35" s="14">
-        <f>G35-H35</f>
-        <v>1</v>
-      </c>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J37" s="4">
-        <v>8</v>
-      </c>
+      <c r="G37" s="14">
+        <v>4</v>
+      </c>
+      <c r="H37" s="14">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f>G37-H37</f>
+        <v>4</v>
+      </c>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E38" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" s="14" t="s">
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="14">
-        <v>4</v>
-      </c>
-      <c r="H38" s="14">
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
         <f>G38-H38</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G39">
-        <v>3</v>
-      </c>
-      <c r="H39">
-        <v>3</v>
-      </c>
-      <c r="I39">
+      <c r="G39" s="14">
+        <v>3</v>
+      </c>
+      <c r="H39" s="14">
+        <v>0</v>
+      </c>
+      <c r="I39" s="14">
         <f>G39-H39</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G40" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H40" s="14">
         <v>0</v>
       </c>
       <c r="I40" s="14">
         <f>G40-H40</f>
-        <v>3</v>
-      </c>
-      <c r="J40" s="4"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G41" s="14">
         <v>1</v>
@@ -2969,53 +2985,54 @@
         <f>G41-H41</f>
         <v>1</v>
       </c>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E42" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="14">
-        <v>1</v>
-      </c>
-      <c r="H42" s="14">
-        <v>0</v>
-      </c>
-      <c r="I42" s="14">
-        <f>G42-H42</f>
-        <v>1</v>
-      </c>
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J43" s="4"/>
+      <c r="E43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J43" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J44" s="4">
-        <v>7</v>
-      </c>
+      <c r="E44" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f>G44-H44</f>
+        <v>2</v>
+      </c>
+      <c r="J44" s="4"/>
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" t="s">
-        <v>6</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
+      <c r="E45" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="14">
+        <v>1</v>
+      </c>
+      <c r="H45" s="14">
+        <v>0</v>
+      </c>
+      <c r="I45" s="14">
         <f>G45-H45</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" s="4"/>
     </row>
@@ -3024,7 +3041,7 @@
         <v>47</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G46" s="14">
         <v>1</v>
@@ -3038,58 +3055,58 @@
       </c>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E47" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="14">
-        <v>1</v>
-      </c>
-      <c r="H47" s="14">
-        <v>0</v>
-      </c>
-      <c r="I47" s="14">
-        <f>G47-H47</f>
-        <v>1</v>
-      </c>
-      <c r="J47" s="4"/>
+    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J48" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J49" s="4">
-        <v>7</v>
-      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <f>G49-H49</f>
+        <v>2</v>
+      </c>
+      <c r="J49" s="5"/>
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
+      <c r="E50" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="14">
+        <v>1</v>
+      </c>
+      <c r="H50" s="14">
+        <v>0</v>
+      </c>
+      <c r="I50" s="14">
         <f>G50-H50</f>
-        <v>2</v>
-      </c>
-      <c r="J50" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="J50" s="15"/>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E51" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G51" s="14">
         <v>1</v>
@@ -3104,79 +3121,79 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E52" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="14">
-        <v>1</v>
-      </c>
-      <c r="H52" s="14">
-        <v>0</v>
-      </c>
-      <c r="I52" s="14">
-        <f>G52-H52</f>
-        <v>1</v>
-      </c>
-      <c r="J52" s="15"/>
+      <c r="J52" s="5"/>
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J53" s="5"/>
+      <c r="E53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E54" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J54" s="4">
-        <v>7</v>
-      </c>
+      <c r="E54" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f>G54-H54</f>
+        <v>5</v>
+      </c>
+      <c r="J54" s="5"/>
     </row>
     <row r="55" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E55" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G55" s="14">
-        <v>5</v>
-      </c>
-      <c r="H55" s="14">
-        <v>0</v>
-      </c>
-      <c r="I55" s="14">
+      <c r="E55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
         <f>G55-H55</f>
-        <v>5</v>
-      </c>
-      <c r="J55" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="J55" s="5"/>
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56">
-        <v>2</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
+      <c r="E56" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="14">
+        <v>1</v>
+      </c>
+      <c r="H56" s="14">
+        <v>0</v>
+      </c>
+      <c r="I56" s="14">
         <f>G56-H56</f>
-        <v>2</v>
-      </c>
-      <c r="J56" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="J56" s="5"/>
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E57" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G57" s="14">
         <v>1</v>
@@ -3188,52 +3205,58 @@
         <f>G57-H57</f>
         <v>1</v>
       </c>
-      <c r="J57" s="14"/>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E58" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" s="14">
-        <v>1</v>
-      </c>
-      <c r="H58" s="14">
-        <v>0</v>
-      </c>
-      <c r="I58" s="14">
-        <f>G58-H58</f>
-        <v>1</v>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+    </row>
+    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J59" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J60" s="5">
-        <v>2</v>
-      </c>
+      <c r="E60" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="14">
+        <v>5</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <f t="shared" ref="I60:I61" si="0">G60-H60</f>
+        <v>5</v>
+      </c>
+      <c r="J60" s="5"/>
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E61" t="s">
-        <v>72</v>
-      </c>
-      <c r="F61" t="s">
-        <v>6</v>
-      </c>
-      <c r="G61">
-        <v>5</v>
+      <c r="E61" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="14">
+        <v>3</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61">
-        <f>G61-H61</f>
-        <v>5</v>
-      </c>
-      <c r="J61" s="5"/>
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
@@ -3252,7 +3275,6 @@
         <f>G62-H62</f>
         <v>2</v>
       </c>
-      <c r="J62" s="5"/>
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E63" s="14" t="s">
@@ -3271,7 +3293,6 @@
         <f>G63-H63</f>
         <v>1</v>
       </c>
-      <c r="J63" s="5"/>
     </row>
     <row r="64" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E64" s="14" t="s">
@@ -3291,16 +3312,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-    </row>
     <row r="66" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E66" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J66" s="5">
         <v>6</v>
@@ -3311,7 +3325,7 @@
         <v>72</v>
       </c>
       <c r="F67" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G67" s="14">
         <v>5</v>
@@ -3320,17 +3334,16 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I68" si="0">G67-H67</f>
+        <f t="shared" ref="I67:I68" si="1">G67-H67</f>
         <v>5</v>
       </c>
-      <c r="J67" s="5"/>
     </row>
     <row r="68" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E68" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F68" s="14" t="s">
-        <v>6</v>
+      <c r="F68" t="s">
+        <v>9</v>
       </c>
       <c r="G68" s="14">
         <v>3</v>
@@ -3339,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3348,7 +3361,7 @@
         <v>46</v>
       </c>
       <c r="F69" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G69">
         <v>2</v>
@@ -3366,7 +3379,7 @@
         <v>47</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G70" s="14">
         <v>1</v>
@@ -3384,7 +3397,7 @@
         <v>47</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G71" s="14">
         <v>1</v>
@@ -3399,10 +3412,10 @@
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" s="1" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="J73" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="5:10" x14ac:dyDescent="0.25">
@@ -3410,7 +3423,7 @@
         <v>72</v>
       </c>
       <c r="F74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G74" s="14">
         <v>5</v>
@@ -3419,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="I74">
-        <f t="shared" ref="I74:I75" si="1">G74-H74</f>
+        <f t="shared" ref="I74:I75" si="2">G74-H74</f>
         <v>5</v>
       </c>
     </row>
@@ -3428,7 +3441,7 @@
         <v>45</v>
       </c>
       <c r="F75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G75" s="14">
         <v>3</v>
@@ -3437,16 +3450,17 @@
         <v>0</v>
       </c>
       <c r="I75">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J75" s="5"/>
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>46</v>
       </c>
       <c r="F76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G76">
         <v>2</v>
@@ -3464,7 +3478,7 @@
         <v>47</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G77" s="14">
         <v>1</v>
@@ -3482,7 +3496,7 @@
         <v>47</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G78" s="14">
         <v>1</v>
@@ -3495,93 +3509,99 @@
         <v>1</v>
       </c>
     </row>
+    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+    </row>
     <row r="80" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E80" s="1" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="J80" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E81" s="14" t="s">
         <v>72</v>
       </c>
       <c r="F81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G81" s="14">
-        <v>5</v>
-      </c>
-      <c r="H81">
+        <v>2</v>
+      </c>
+      <c r="H81" s="14">
         <v>0</v>
       </c>
       <c r="I81">
-        <f t="shared" ref="I81:I82" si="2">G81-H81</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
+        <f>G81-H81</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E82" s="14" t="s">
         <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G82" s="14">
-        <v>3</v>
-      </c>
-      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="H82" s="14">
         <v>0</v>
       </c>
       <c r="I82">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I82:I85" si="3">G82-H82</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
         <v>46</v>
       </c>
       <c r="F83" t="s">
-        <v>8</v>
-      </c>
-      <c r="G83">
-        <v>2</v>
-      </c>
-      <c r="H83">
+        <v>6</v>
+      </c>
+      <c r="G83" s="14">
+        <v>2</v>
+      </c>
+      <c r="H83" s="14">
         <v>0</v>
       </c>
       <c r="I83">
-        <f>G83-H83</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E84" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F84" s="14" t="s">
-        <v>6</v>
+      <c r="F84" t="s">
+        <v>9</v>
       </c>
       <c r="G84" s="14">
         <v>1</v>
       </c>
-      <c r="H84" s="14">
-        <v>0</v>
-      </c>
-      <c r="I84" s="14">
-        <f>G84-H84</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E85" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F85" s="14" t="s">
-        <v>8</v>
+      <c r="F85" t="s">
+        <v>6</v>
       </c>
       <c r="G85" s="14">
         <v>1</v>
@@ -3589,149 +3609,138 @@
       <c r="H85" s="14">
         <v>0</v>
       </c>
-      <c r="I85" s="14">
-        <f>G85-H85</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-    </row>
-    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E87" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J87" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E88" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="F88" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E90" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J90" s="5">
+        <v>9</v>
+      </c>
+      <c r="G88" s="14">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <f>G88-H88</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>46</v>
+      </c>
+      <c r="F89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <f>G89-H89</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E90" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G90" s="14">
+        <v>1</v>
+      </c>
+      <c r="H90" s="14">
+        <v>0</v>
+      </c>
+      <c r="I90" s="14">
+        <f>G90-H90</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E91" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F91" t="s">
+        <v>47</v>
+      </c>
+      <c r="F91" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G91" s="14">
+        <v>1</v>
+      </c>
+      <c r="H91" s="14">
+        <v>0</v>
+      </c>
+      <c r="I91" s="14">
+        <f>G91-H91</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E93" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F93" t="s">
+        <v>8</v>
+      </c>
+      <c r="G93" s="14">
         <v>7</v>
       </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91">
-        <f t="shared" ref="I91" si="3">G91-H91</f>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <f>G93-H93</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E92" t="s">
-        <v>46</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="J93" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E95" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F95" t="s">
         <v>9</v>
       </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92">
-        <f>G92-H92</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E93" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F93" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G93" s="14">
-        <v>1</v>
-      </c>
-      <c r="H93" s="14">
-        <v>0</v>
-      </c>
-      <c r="I93" s="14">
-        <f>G93-H93</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E94" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F94" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G94" s="14">
-        <v>1</v>
-      </c>
-      <c r="H94" s="14">
-        <v>0</v>
-      </c>
-      <c r="I94" s="14">
-        <f>G94-H94</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E96" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J96" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E98" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J98" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F99" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="L101" s="20"/>
-      <c r="M101" s="20"/>
-    </row>
-    <row r="102" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="L102" s="20"/>
-      <c r="M102" s="20"/>
-    </row>
-    <row r="105" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E105" s="18"/>
-    </row>
-    <row r="106" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E106" s="1"/>
-      <c r="J106" s="4"/>
-    </row>
-    <row r="107" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="J107" s="4"/>
+      <c r="G95" s="14">
+        <v>6</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <f>G95-H95</f>
+        <v>6</v>
+      </c>
+      <c r="J95" s="5">
+        <v>8</v>
+      </c>
+      <c r="L95" s="20"/>
+      <c r="M95" s="20"/>
+    </row>
+    <row r="96" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="L96" s="20"/>
+      <c r="M96" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3744,7 +3753,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3838,15 +3847,20 @@
       <c r="A9" s="18" t="s">
         <v>67</v>
       </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="14" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="4"/>
@@ -3854,6 +3868,9 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>66</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3864,10 +3881,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G5:G6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3893,7 +3910,20 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>